<commit_message>
finished initial work on react router. Also, created a new endpoint to pull filtered/shuffled questions from backend, given a quizId and quiz configurations in req body. Finally, also created a new endpoint to allow for new quizzes to be added to repo (added react design patterns and html5)
</commit_message>
<xml_diff>
--- a/quiz-content/quiz-template.xlsx
+++ b/quiz-content/quiz-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbuongiovanni/Documents/VSchool/quizzly/quiz-content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbuongiovanni/Documents/VSchool/open-quizzly/quiz-content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A499537-29DA-C248-A244-9E189CE3E29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30C3BDB-EE39-5949-BA5F-AFEF649662E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38520" yWindow="500" windowWidth="38400" windowHeight="20180" xr2:uid="{E2CC4BDD-25FB-B04B-8F58-81BCD1F07F5F}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{E2CC4BDD-25FB-B04B-8F58-81BCD1F07F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Patterns in React" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="214">
   <si>
     <t>quizName</t>
   </si>
@@ -454,12 +454,6 @@
   </si>
   <si>
     <t>Semantic tags</t>
-  </si>
-  <si>
-    <t>HTML6</t>
-  </si>
-  <si>
-    <t>HTML7</t>
   </si>
   <si>
     <t>Which of the following tag insists to have a value in an input control in HTML5?</t>
@@ -1152,7 +1146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DC4991-AB7F-2B41-ACAD-4F0A86441FD5}">
   <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1193,7 +1187,7 @@
         <v>95</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
@@ -1213,7 +1207,7 @@
         <v>95</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -1233,7 +1227,7 @@
         <v>95</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
@@ -1379,10 +1373,10 @@
         <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1399,10 +1393,10 @@
         <v>14</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1419,7 +1413,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>21</v>
@@ -2033,13 +2027,13 @@
         <v>95</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>44</v>
@@ -2053,13 +2047,13 @@
         <v>95</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>31</v>
@@ -2073,13 +2067,13 @@
         <v>95</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>119</v>
@@ -2093,16 +2087,16 @@
         <v>95</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -2113,10 +2107,10 @@
         <v>95</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>60</v>
@@ -2133,10 +2127,10 @@
         <v>95</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>60</v>
@@ -2153,13 +2147,13 @@
         <v>95</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>64</v>
@@ -2173,13 +2167,13 @@
         <v>95</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>65</v>
@@ -2193,13 +2187,13 @@
         <v>95</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>66</v>
@@ -2262,7 +2256,7 @@
         <v>67</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2279,7 +2273,7 @@
         <v>70</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>72</v>
@@ -2299,7 +2293,7 @@
         <v>70</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>73</v>
@@ -2319,10 +2313,10 @@
         <v>70</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -2502,7 +2496,7 @@
         <v>83</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -2782,7 +2776,7 @@
         <v>104</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -2993,7 +2987,7 @@
         <v>95</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>124</v>
@@ -3013,7 +3007,7 @@
         <v>95</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>124</v>
@@ -3033,7 +3027,7 @@
         <v>95</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>124</v>
@@ -3053,7 +3047,7 @@
         <v>95</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>127</v>
@@ -3062,7 +3056,7 @@
         <v>128</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3073,7 +3067,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>127</v>
@@ -3093,7 +3087,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>127</v>
@@ -3182,7 +3176,7 @@
         <v>126</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3202,7 +3196,7 @@
         <v>126</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3603,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0106E64C-4554-9749-88C7-E53A7DF75609}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3645,16 +3639,16 @@
         <v>132</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3665,16 +3659,16 @@
         <v>132</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3685,16 +3679,16 @@
         <v>132</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3705,16 +3699,16 @@
         <v>132</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3725,16 +3719,16 @@
         <v>132</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3745,16 +3739,16 @@
         <v>132</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E7" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3765,16 +3759,16 @@
         <v>132</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3785,16 +3779,16 @@
         <v>132</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3805,16 +3799,16 @@
         <v>132</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3825,16 +3819,16 @@
         <v>132</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3845,16 +3839,16 @@
         <v>132</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>157</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3865,16 +3859,16 @@
         <v>132</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3885,16 +3879,16 @@
         <v>132</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3905,16 +3899,16 @@
         <v>132</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3925,16 +3919,16 @@
         <v>132</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3945,16 +3939,16 @@
         <v>132</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3965,16 +3959,16 @@
         <v>132</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3985,16 +3979,16 @@
         <v>132</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4008,13 +4002,13 @@
         <v>133</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4022,19 +4016,19 @@
         <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4042,19 +4036,19 @@
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4068,13 +4062,13 @@
         <v>133</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4082,19 +4076,19 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4102,19 +4096,19 @@
         <v>2</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -4128,13 +4122,13 @@
         <v>133</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -4142,19 +4136,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -4162,19 +4156,19 @@
         <v>2</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4188,13 +4182,13 @@
         <v>133</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4202,19 +4196,19 @@
         <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4222,19 +4216,19 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -4248,13 +4242,13 @@
         <v>133</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -4262,19 +4256,19 @@
         <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -4282,19 +4276,19 @@
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4308,13 +4302,13 @@
         <v>133</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4322,19 +4316,19 @@
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4342,19 +4336,19 @@
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4368,13 +4362,13 @@
         <v>133</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4382,19 +4376,19 @@
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4402,19 +4396,19 @@
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4428,13 +4422,13 @@
         <v>133</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4442,19 +4436,19 @@
         <v>2</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4462,19 +4456,19 @@
         <v>2</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4488,13 +4482,13 @@
         <v>133</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4502,19 +4496,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4522,19 +4516,19 @@
         <v>2</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4548,13 +4542,13 @@
         <v>133</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4562,19 +4556,19 @@
         <v>2</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4582,22 +4576,22 @@
         <v>2</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>2</v>
       </c>
@@ -4608,53 +4602,53 @@
         <v>133</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished initial design/styling of App. Also made spot changes to html structure/classNames
</commit_message>
<xml_diff>
--- a/quiz-content/quiz-template.xlsx
+++ b/quiz-content/quiz-template.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbuongiovanni/Documents/VSchool/open-quizzly/quiz-content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802053A5-1328-524A-A69E-D403D580CE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA752CC-3582-E54D-B861-4BC8C8D953EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="20180" xr2:uid="{E2CC4BDD-25FB-B04B-8F58-81BCD1F07F5F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{E2CC4BDD-25FB-B04B-8F58-81BCD1F07F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Patterns in React" sheetId="1" r:id="rId1"/>
-    <sheet name="HTML5" sheetId="3" r:id="rId2"/>
+    <sheet name="JavaScript" sheetId="4" r:id="rId2"/>
+    <sheet name="HTML5" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Design Patterns in React'!$A$1:$G$109</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">HTML5!$A$1:$F$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">HTML5!$A$1:$F$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="326">
   <si>
     <t>quizName</t>
   </si>
@@ -745,6 +746,347 @@
   </si>
   <si>
     <t>Creational patterns facilitate the management of newly created objects, thereby allowing an increase in flexibility and reuse of existing code. Structural patterns explain how to assemble objects and classes into larger structures, while keeping these structures flexible and efficient. Behavioral patterns take care of effective communication and assignment of responsibilities between objects.</t>
+  </si>
+  <si>
+    <t>JavaScript - Basics</t>
+  </si>
+  <si>
+    <t>Variable and Values</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>What happens when you concatenate the empty string with NaN?</t>
+  </si>
+  <si>
+    <t>What happens when you concatenate the empty string with Infinity?</t>
+  </si>
+  <si>
+    <t>What happens when you concatenate the empty string with false?</t>
+  </si>
+  <si>
+    <t>What happens when you concatenate the empty string with true?</t>
+  </si>
+  <si>
+    <t>What happens when you concatenate the empty string with null?</t>
+  </si>
+  <si>
+    <t>What happens when you concatenate the empty string with undefined?</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>'NaN'</t>
+  </si>
+  <si>
+    <t>'false'</t>
+  </si>
+  <si>
+    <t>'true'</t>
+  </si>
+  <si>
+    <t>'null'</t>
+  </si>
+  <si>
+    <t>'undefined'</t>
+  </si>
+  <si>
+    <t>'Infinity'</t>
+  </si>
+  <si>
+    <t>What happens when you add 0 with NaN?</t>
+  </si>
+  <si>
+    <t>What happens when you add 0 with Infinity?</t>
+  </si>
+  <si>
+    <t>What happens when you add 0 with false?</t>
+  </si>
+  <si>
+    <t>What happens when you add 0 with true?</t>
+  </si>
+  <si>
+    <t>What happens when you add 0 with null?</t>
+  </si>
+  <si>
+    <t>What happens when you add 0 with undefined?</t>
+  </si>
+  <si>
+    <t>Infinity</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+0 == "0"</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+0 === "0"</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+undefined === undefined</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+NaN === NaN</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+null === null</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+10 * null</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+10 * NaN</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+10 * undefined</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+null == undefined</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+null === undefined</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>Q17</t>
+  </si>
+  <si>
+    <t>Q18</t>
+  </si>
+  <si>
+    <t>Q19</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>Q21</t>
+  </si>
+  <si>
+    <t>Q22</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+null == 0</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+null === 0</t>
+  </si>
+  <si>
+    <t>What is the correct syntax to reference an external JavaScript Script from an HTML file?</t>
+  </si>
+  <si>
+    <t>&lt;script src="myscripts.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+typeof NaN</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>typeof typeof 1</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+const numbers = [33, 2, 8]; 
+numbers.sort();
+console.log(numbers[1])</t>
+  </si>
+  <si>
+    <t>Syntax</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+let a = 1;
+a = 2;
+console.log(a);</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+const a = 1;
+a = 2;
+console.log(a);</t>
+  </si>
+  <si>
+    <t>A TypeError will be thrown</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+console.log(square(2));
+const square = function(x) {
+  return x * x
+};</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+console.log(square(2));
+function square(x) {
+  return x * x
+};</t>
+  </si>
+  <si>
+    <t>A ReferenceError will be thrown</t>
+  </si>
+  <si>
+    <t>Which of the following will write the message “Hello World!” in an alert box?</t>
+  </si>
+  <si>
+    <t>alert(“Hello DataFlair!”);</t>
+  </si>
+  <si>
+    <t>Which is the correct JavaScript syntax to change the HTML content given below?
+&lt;p id=”test”&gt;Hello World!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> document.getElementById(“test”).innerHTML = “Hello World!”;</t>
+  </si>
+  <si>
+    <t>Pete, Barb, Lenny, and Julie</t>
+  </si>
+  <si>
+    <t>In what order will the names appear?
+function shoutOut() {
+    console.log("Pete");
+    setTimeout(function() {console.log("Julie")}, 1000);
+    setTimeout(function() {console.log("Barb")}, 0);
+    console.log("Lenny");
+}
+shoutOut()</t>
+  </si>
+  <si>
+    <t>Pete, Lenny, Barb, and Julie</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+{} === {}</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+{} == {}</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+[] == []</t>
+  </si>
+  <si>
+    <t>What is the result of: 
+[] === []</t>
+  </si>
+  <si>
+    <t>What are the data types in JavaScript, based on the typeof operator</t>
+  </si>
+  <si>
+    <t>number, string, boolean, object, symbol, and undefined</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>objects</t>
+  </si>
+  <si>
+    <t>What are the non-primitive type(s)</t>
+  </si>
+  <si>
+    <t>What are the primitive types?</t>
+  </si>
+  <si>
+    <t>number, string, boolean, NULL, undefined, and Symbol.</t>
+  </si>
+  <si>
+    <t>number, string, boolean, NULL, and undefined.</t>
+  </si>
+  <si>
+    <t>What is 'Hoisting'?</t>
+  </si>
+  <si>
+    <t>Default behavior where variables and function declarations are moved to top of script.</t>
+  </si>
+  <si>
+    <t>What is the difference between "==" and "==="?</t>
+  </si>
+  <si>
+    <t>Double equals is a weak evaluation which only compares values, whereas triple equal compares values and types.</t>
+  </si>
+  <si>
+    <t>What are the truthy values?</t>
+  </si>
+  <si>
+    <t>All values except false, 0, 0n, -0, “”, null, undefined, and NaN</t>
+  </si>
+  <si>
+    <t>"goodbye"</t>
+  </si>
+  <si>
+    <t>"hello"</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+console.log("hello!" || "goodbye")</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+console.log("hello!" &amp;&amp; "goodbye")</t>
   </si>
 </sst>
 </file>
@@ -833,7 +1175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -878,6 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1194,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DC4991-AB7F-2B41-ACAD-4F0A86441FD5}">
   <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -4123,6 +4466,846 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F4E592-B51F-4B40-A294-DF24242C3153}">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="130" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="68" customWidth="1"/>
+    <col min="6" max="6" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F5" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F14" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F15" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F16" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F17" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F30" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="F31" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="C32" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F32" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="C33" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F33">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="C34" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F35" t="s">
+        <v>293</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="C36" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F36" t="s">
+        <v>296</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="C37" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C38" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="F38" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C39" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="F39" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="C40" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F40" t="s">
+        <v>303</v>
+      </c>
+      <c r="G40" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C41" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F41" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C42" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="F42" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C43" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="F43" t="s">
+        <v>314</v>
+      </c>
+      <c r="G43" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C44" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F44" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C45" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="F45" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C46" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="F46" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C47" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="F47" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C48" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="F48" t="s">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0106E64C-4554-9749-88C7-E53A7DF75609}">
   <dimension ref="A1:F52"/>
   <sheetViews>

</xml_diff>

<commit_message>
refactored/broke out existing components under the HistoricalResults component (and it's children)
</commit_message>
<xml_diff>
--- a/quiz-content/quiz-template.xlsx
+++ b/quiz-content/quiz-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbuongiovanni/Documents/VSchool/open-quizzly/quiz-content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA752CC-3582-E54D-B861-4BC8C8D953EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5219ACF-0AB9-D742-958A-08029088F24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{E2CC4BDD-25FB-B04B-8F58-81BCD1F07F5F}"/>
+    <workbookView xWindow="-44980" yWindow="1140" windowWidth="38400" windowHeight="20180" activeTab="1" xr2:uid="{E2CC4BDD-25FB-B04B-8F58-81BCD1F07F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Patterns in React" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Design Patterns in React'!$A$1:$G$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">HTML5!$A$1:$F$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">JavaScript!$A$1:$G$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="387">
   <si>
     <t>quizName</t>
   </si>
@@ -1060,9 +1061,6 @@
     <t>What is 'Hoisting'?</t>
   </si>
   <si>
-    <t>Default behavior where variables and function declarations are moved to top of script.</t>
-  </si>
-  <si>
     <t>What is the difference between "==" and "==="?</t>
   </si>
   <si>
@@ -1070,9 +1068,6 @@
   </si>
   <si>
     <t>What are the truthy values?</t>
-  </si>
-  <si>
-    <t>All values except false, 0, 0n, -0, “”, null, undefined, and NaN</t>
   </si>
   <si>
     <t>"goodbye"</t>
@@ -1087,6 +1082,205 @@
   <si>
     <t>What will be printed to the console:
 console.log("hello!" &amp;&amp; "goodbye")</t>
+  </si>
+  <si>
+    <t>All values except false, 0, 0n, -0, "", null, undefined, and NaN</t>
+  </si>
+  <si>
+    <t>How does the var keyword differ from the let and const keywords with respect to hoisting?</t>
+  </si>
+  <si>
+    <t>Unlike var, variables defined with let and const are not hoisted.</t>
+  </si>
+  <si>
+    <t>Hoisting</t>
+  </si>
+  <si>
+    <t>What are Higher Order Functions?</t>
+  </si>
+  <si>
+    <t>Functions that either take in function(s) one or more parameter and/or returns a function</t>
+  </si>
+  <si>
+    <t>Which of the following are true regarding ES6 Arrow Functions?</t>
+  </si>
+  <si>
+    <t>ES6 Arrow functions can be used to create constructor functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The execution context (or 'this' keyword) of an arrow function is resolved lexically, meaning it gets its value from the outer function or global scope. </t>
+  </si>
+  <si>
+    <t>Functions that take a class as an argument.</t>
+  </si>
+  <si>
+    <t>Which of the following instantiates a new Person object into an object called "student"</t>
+  </si>
+  <si>
+    <t>const student = new Person();</t>
+  </si>
+  <si>
+    <t>What will be printed to the console:
+let animals = ["tiger", "lion", "dog"];
+a[10] = "cat";
+console.log(a.length);</t>
+  </si>
+  <si>
+    <t>What will the following function return:
+() =&gt; {type : "ice cream"}</t>
+  </si>
+  <si>
+    <t>An object with the property "type" that has a value of "ice cream"</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>What is a function whose execution can be suspended and resumed at a later point?</t>
+  </si>
+  <si>
+    <t>Generator Function</t>
+  </si>
+  <si>
+    <t>Async Function</t>
+  </si>
+  <si>
+    <t>Q23</t>
+  </si>
+  <si>
+    <t>Q24</t>
+  </si>
+  <si>
+    <t>Q25</t>
+  </si>
+  <si>
+    <t>Q26</t>
+  </si>
+  <si>
+    <t>Q27</t>
+  </si>
+  <si>
+    <t>Q28</t>
+  </si>
+  <si>
+    <t>Q29</t>
+  </si>
+  <si>
+    <t>Q30</t>
+  </si>
+  <si>
+    <t>Q31</t>
+  </si>
+  <si>
+    <t>Q32</t>
+  </si>
+  <si>
+    <t>Q33</t>
+  </si>
+  <si>
+    <t>Q34</t>
+  </si>
+  <si>
+    <t>Q35</t>
+  </si>
+  <si>
+    <t>Q36</t>
+  </si>
+  <si>
+    <t>Q37</t>
+  </si>
+  <si>
+    <t>Q38</t>
+  </si>
+  <si>
+    <t>Q39</t>
+  </si>
+  <si>
+    <t>Q40</t>
+  </si>
+  <si>
+    <t>Q41</t>
+  </si>
+  <si>
+    <t>Q42</t>
+  </si>
+  <si>
+    <t>Q43</t>
+  </si>
+  <si>
+    <t>Q44</t>
+  </si>
+  <si>
+    <t>Q45</t>
+  </si>
+  <si>
+    <t>Q46</t>
+  </si>
+  <si>
+    <t>Q47</t>
+  </si>
+  <si>
+    <t>Q48</t>
+  </si>
+  <si>
+    <t>Q49</t>
+  </si>
+  <si>
+    <t>Q50</t>
+  </si>
+  <si>
+    <t>Q51</t>
+  </si>
+  <si>
+    <t>Q52</t>
+  </si>
+  <si>
+    <t>Q53</t>
+  </si>
+  <si>
+    <t>Q54</t>
+  </si>
+  <si>
+    <t>Q55</t>
+  </si>
+  <si>
+    <t>What will func2 log to the console?
+var v = 1;
+var func1 = function() {console.log(v)}
+var func2 = function() {
+var v = 2
+funct1()
+}</t>
+  </si>
+  <si>
+    <t>What is the difference between var and let with respect to scoping</t>
+  </si>
+  <si>
+    <t>"let" is block scope whereas "var" is function or globally scoped</t>
+  </si>
+  <si>
+    <t>Default behavior where variables and function declarations are moved to top of script (global) or function (if declared within a function).</t>
+  </si>
+  <si>
+    <t>Unlike var, variables declared with let and const are not initialized with a default when hoisted.</t>
+  </si>
+  <si>
+    <t>What is the difference between 'let' and 'const'</t>
+  </si>
+  <si>
+    <t>A variable defined with the 'let' keyword can be reassigned. Variables defined with 'const' cannot be reassigned.</t>
+  </si>
+  <si>
+    <t>A variable defined with the 'let' keyword can be modified. Variables defined with 'const' cannot be modified.</t>
+  </si>
+  <si>
+    <t>Which of the following are true regarding null and undefined?</t>
+  </si>
+  <si>
+    <t>Null is an object whereas undefined is undefined.</t>
+  </si>
+  <si>
+    <t>Practically speaking, they are the exact same.</t>
   </si>
 </sst>
 </file>
@@ -4467,18 +4661,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F4E592-B51F-4B40-A294-DF24242C3153}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="130" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="5" width="68" customWidth="1"/>
-    <col min="6" max="6" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="126" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -4505,187 +4699,147 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>228</v>
+        <v>310</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>229</v>
+        <v>360</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>308</v>
+      </c>
+      <c r="F2" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>228</v>
+        <v>310</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>236</v>
+        <v>361</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>261</v>
+        <v>312</v>
+      </c>
+      <c r="F3" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>228</v>
+        <v>310</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>237</v>
+        <v>362</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="F4" s="16">
-        <v>0</v>
+        <v>313</v>
+      </c>
+      <c r="F4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G4" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>228</v>
+        <v>138</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>238</v>
+        <v>369</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="F5" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="F5" t="s">
+        <v>329</v>
+      </c>
+      <c r="G5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>228</v>
+        <v>138</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>239</v>
+        <v>372</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="F6" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>228</v>
+        <v>138</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>240</v>
+        <v>374</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>248</v>
+        <v>340</v>
+      </c>
+      <c r="F7" t="s">
+        <v>341</v>
+      </c>
+      <c r="G7" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>241</v>
+        <v>138</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="F8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
-        <v>228</v>
+        <v>327</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>242</v>
+        <v>368</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>254</v>
+        <v>325</v>
+      </c>
+      <c r="F9" t="s">
+        <v>380</v>
+      </c>
+      <c r="G9" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>243</v>
+        <v>370</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="F10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -4693,331 +4847,270 @@
         <v>227</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>244</v>
+        <v>349</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="F11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>245</v>
+        <v>352</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="F12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>246</v>
+        <v>353</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>290</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>354</v>
+      </c>
       <c r="E14" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="F14" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="F14" t="s">
+        <v>293</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>290</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>355</v>
+      </c>
       <c r="E15" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="F15" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="F15" t="s">
+        <v>296</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>290</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="E16" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="F16" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>290</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="E17" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F17" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="F17" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>247</v>
+        <v>358</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="F18" t="b">
+        <v>299</v>
+      </c>
+      <c r="F18" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F19" t="s">
+        <v>303</v>
+      </c>
+      <c r="G19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C20" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F20" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="F21" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C22" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F22" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C23" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F23" t="s">
+        <v>321</v>
+      </c>
+      <c r="G23" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C24" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="F24" t="s">
+        <v>320</v>
+      </c>
+      <c r="G24" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C25" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="F25" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="F26" t="s">
+        <v>339</v>
+      </c>
+      <c r="G26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="C27" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="F24" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="F25" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -5028,16 +5121,17 @@
         <v>228</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>279</v>
+        <v>229</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
@@ -5048,16 +5142,16 @@
         <v>228</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>280</v>
+        <v>236</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
@@ -5065,16 +5159,19 @@
         <v>227</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>138</v>
+        <v>228</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="F30" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -5085,221 +5182,563 @@
         <v>228</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>280</v>
+        <v>238</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="F31" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="F31" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>227</v>
+      </c>
       <c r="C32" s="2" t="s">
         <v>228</v>
       </c>
+      <c r="D32" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="E32" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F32" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F40" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F41" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F42" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F43" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F50" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F51" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="F56" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C57" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F57" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="3:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="C33" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="F33">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="C34" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="G34" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="35" spans="3:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="C35" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="F35" t="s">
-        <v>293</v>
-      </c>
-      <c r="G35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="C36" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="F36" t="s">
-        <v>296</v>
-      </c>
-      <c r="G36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="C37" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="F37">
-        <v>4</v>
-      </c>
-      <c r="G37" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="C38" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="F38" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="C39" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="F39" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="C40" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="F40" t="s">
-        <v>303</v>
-      </c>
-      <c r="G40" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="C41" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="F41" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="42" spans="3:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="C42" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="F42" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="43" spans="3:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="C43" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="F43" t="s">
-        <v>314</v>
-      </c>
-      <c r="G43" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="44" spans="3:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="C44" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="F44" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="45" spans="3:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="C45" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="F45" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="46" spans="3:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="C46" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="F46" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="47" spans="3:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="C47" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="F47" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="48" spans="3:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="C48" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="F48" t="s">
-        <v>322</v>
+    <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C58" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="F58" t="s">
+        <v>382</v>
+      </c>
+      <c r="G58" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C59" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="F59" t="s">
+        <v>385</v>
+      </c>
+      <c r="G59" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G57" xr:uid="{F1F4E592-B51F-4B40-A294-DF24242C3153}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G57">
+      <sortCondition ref="C1:C57"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>